<commit_message>
Added KLD and AER
</commit_message>
<xml_diff>
--- a/app/_spreadsheets/ogw.xlsx
+++ b/app/_spreadsheets/ogw.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\matt\Dropbox (Mktg)\Personal - Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="20115" windowHeight="12015"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ogw!$A$1:$M$185</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1746,7 +1751,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1859,7 +1864,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1894,7 +1899,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2106,22 +2111,23 @@
   <dimension ref="A1:M185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="0.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" style="4" customWidth="1"/>
     <col min="9" max="10" width="9.85546875" style="3" customWidth="1"/>
-    <col min="11" max="13" width="8.7109375" style="3" customWidth="1"/>
+    <col min="11" max="12" width="8.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="3" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -2194,6 +2200,16 @@
       <c r="J2" s="3">
         <v>8</v>
       </c>
+      <c r="K2" s="3">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3">
+        <f>_xlfn.CEILING.MATH(AVERAGE(K2,L2))</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -2223,6 +2239,16 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
+      <c r="K3" s="3">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M66" si="0">_xlfn.CEILING.MATH(AVERAGE(K3,L3))</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -2251,6 +2277,16 @@
       </c>
       <c r="J4" s="3">
         <v>5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>14</v>
+      </c>
+      <c r="L4" s="3">
+        <v>14</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2284,6 +2320,16 @@
       <c r="J5" s="3">
         <v>12</v>
       </c>
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -2313,6 +2359,16 @@
       <c r="J6" s="3">
         <v>5</v>
       </c>
+      <c r="K6" s="3">
+        <v>8</v>
+      </c>
+      <c r="L6" s="3">
+        <v>8</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -2342,6 +2398,16 @@
       <c r="J7" s="3">
         <v>2</v>
       </c>
+      <c r="K7" s="3">
+        <v>12</v>
+      </c>
+      <c r="L7" s="3">
+        <v>14</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -2374,6 +2440,16 @@
       <c r="J8" s="3">
         <v>5</v>
       </c>
+      <c r="K8" s="3">
+        <v>13</v>
+      </c>
+      <c r="L8" s="3">
+        <v>13</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -2397,6 +2473,16 @@
       <c r="H9" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="K9" s="3">
+        <v>9</v>
+      </c>
+      <c r="L9" s="3">
+        <v>9</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -2426,8 +2512,18 @@
       <c r="J10" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="K10" s="3">
+        <v>12</v>
+      </c>
+      <c r="L10" s="3">
+        <v>12</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2458,8 +2554,18 @@
       <c r="J11" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3">
+        <v>8</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2490,8 +2596,18 @@
       <c r="J12" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="K12" s="3">
+        <v>7</v>
+      </c>
+      <c r="L12" s="3">
+        <v>7</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2513,8 +2629,18 @@
       <c r="H13" s="4" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2545,8 +2671,18 @@
       <c r="J14" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="K14" s="3">
+        <v>15</v>
+      </c>
+      <c r="L14" s="3">
+        <v>15</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2577,8 +2713,18 @@
       <c r="J15" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="3">
+        <v>7</v>
+      </c>
+      <c r="L15" s="3">
+        <v>7</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2600,8 +2746,18 @@
       <c r="H16" s="4" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K16" s="3">
+        <v>9</v>
+      </c>
+      <c r="L16" s="3">
+        <v>9</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2623,8 +2779,18 @@
       <c r="H17" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2</v>
+      </c>
+      <c r="M17" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2646,8 +2812,18 @@
       <c r="H18" s="4" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K18" s="3">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3">
+        <v>5</v>
+      </c>
+      <c r="M18" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2678,8 +2854,18 @@
       <c r="J19" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K19" s="3">
+        <v>8</v>
+      </c>
+      <c r="L19" s="3">
+        <v>8</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2707,8 +2893,18 @@
       <c r="J20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="3">
+        <v>12</v>
+      </c>
+      <c r="L20" s="3">
+        <v>12</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2730,8 +2926,18 @@
       <c r="H21" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K21" s="3">
+        <v>11</v>
+      </c>
+      <c r="L21" s="3">
+        <v>11</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2756,8 +2962,18 @@
       <c r="H22" s="4" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22" s="3">
+        <v>4</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2779,8 +2995,18 @@
       <c r="H23" s="4" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="3">
+        <v>11</v>
+      </c>
+      <c r="L23" s="3">
+        <v>11</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2808,8 +3034,18 @@
       <c r="J24" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="3">
+        <v>8</v>
+      </c>
+      <c r="L24" s="3">
+        <v>8</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2837,8 +3073,18 @@
       <c r="J25" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K25" s="3">
+        <v>9</v>
+      </c>
+      <c r="L25" s="3">
+        <v>9</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2869,8 +3115,18 @@
       <c r="J26" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="3">
+        <v>15</v>
+      </c>
+      <c r="L26" s="3">
+        <v>15</v>
+      </c>
+      <c r="M26" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2895,8 +3151,18 @@
       <c r="H27" s="4" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="3">
+        <v>8</v>
+      </c>
+      <c r="L27" s="3">
+        <v>8</v>
+      </c>
+      <c r="M27" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2927,8 +3193,18 @@
       <c r="J28" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="3">
+        <v>8</v>
+      </c>
+      <c r="L28" s="3">
+        <v>7</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2953,8 +3229,18 @@
       <c r="H29" s="4" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K29" s="3">
+        <v>5</v>
+      </c>
+      <c r="L29" s="3">
+        <v>5</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2985,8 +3271,18 @@
       <c r="J30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K30" s="3">
+        <v>13</v>
+      </c>
+      <c r="L30" s="3">
+        <v>13</v>
+      </c>
+      <c r="M30" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3008,8 +3304,18 @@
       <c r="H31" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K31" s="3">
+        <v>7</v>
+      </c>
+      <c r="L31" s="3">
+        <v>7</v>
+      </c>
+      <c r="M31" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3040,8 +3346,18 @@
       <c r="J32" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K32" s="3">
+        <v>8</v>
+      </c>
+      <c r="L32" s="3">
+        <v>8</v>
+      </c>
+      <c r="M32" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3072,8 +3388,18 @@
       <c r="J33" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="3">
+        <v>11</v>
+      </c>
+      <c r="L33" s="3">
+        <v>11</v>
+      </c>
+      <c r="M33" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3095,8 +3421,18 @@
       <c r="H34" s="4" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K34" s="3">
+        <v>8</v>
+      </c>
+      <c r="L34" s="3">
+        <v>8</v>
+      </c>
+      <c r="M34" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3121,8 +3457,18 @@
       <c r="H35" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K35" s="3">
+        <v>5</v>
+      </c>
+      <c r="L35" s="3">
+        <v>7</v>
+      </c>
+      <c r="M35" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3153,8 +3499,18 @@
       <c r="J36" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K36" s="3">
+        <v>8</v>
+      </c>
+      <c r="L36" s="3">
+        <v>6</v>
+      </c>
+      <c r="M36" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3185,8 +3541,18 @@
       <c r="J37" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K37" s="3">
+        <v>9</v>
+      </c>
+      <c r="L37" s="3">
+        <v>9</v>
+      </c>
+      <c r="M37" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3214,8 +3580,18 @@
       <c r="J38" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K38" s="3">
+        <v>8</v>
+      </c>
+      <c r="L38" s="3">
+        <v>8</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3246,8 +3622,18 @@
       <c r="J39" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K39" s="3">
+        <v>2</v>
+      </c>
+      <c r="L39" s="3">
+        <v>2</v>
+      </c>
+      <c r="M39" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3278,8 +3664,18 @@
       <c r="J40" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K40" s="3">
+        <v>10</v>
+      </c>
+      <c r="L40" s="3">
+        <v>9</v>
+      </c>
+      <c r="M40" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3304,8 +3700,18 @@
       <c r="H41" s="4" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="3">
+        <v>2</v>
+      </c>
+      <c r="L41" s="3">
+        <v>5</v>
+      </c>
+      <c r="M41" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3336,8 +3742,18 @@
       <c r="J42" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K42" s="3">
+        <v>10</v>
+      </c>
+      <c r="L42" s="3">
+        <v>11</v>
+      </c>
+      <c r="M42" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3368,8 +3784,18 @@
       <c r="J43" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K43" s="3">
+        <v>10</v>
+      </c>
+      <c r="L43" s="3">
+        <v>10</v>
+      </c>
+      <c r="M43" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3400,8 +3826,18 @@
       <c r="J44" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K44" s="3">
+        <v>13</v>
+      </c>
+      <c r="L44" s="3">
+        <v>13</v>
+      </c>
+      <c r="M44" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3432,8 +3868,18 @@
       <c r="J45" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K45" s="3">
+        <v>10</v>
+      </c>
+      <c r="L45" s="3">
+        <v>10</v>
+      </c>
+      <c r="M45" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3464,8 +3910,18 @@
       <c r="J46" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="3">
+        <v>9</v>
+      </c>
+      <c r="L46" s="3">
+        <v>9</v>
+      </c>
+      <c r="M46" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3496,8 +3952,18 @@
       <c r="J47" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K47" s="3">
+        <v>6</v>
+      </c>
+      <c r="L47" s="3">
+        <v>7</v>
+      </c>
+      <c r="M47" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3522,8 +3988,18 @@
       <c r="H48" s="4" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K48" s="3">
+        <v>5</v>
+      </c>
+      <c r="L48" s="3">
+        <v>5</v>
+      </c>
+      <c r="M48" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3554,8 +4030,18 @@
       <c r="J49" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K49" s="3">
+        <v>10</v>
+      </c>
+      <c r="L49" s="3">
+        <v>10</v>
+      </c>
+      <c r="M49" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3580,8 +4066,18 @@
       <c r="H50" s="4" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="3">
+        <v>2</v>
+      </c>
+      <c r="L50" s="3">
+        <v>2</v>
+      </c>
+      <c r="M50" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3606,8 +4102,18 @@
       <c r="J51" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K51" s="3">
+        <v>6</v>
+      </c>
+      <c r="L51" s="3">
+        <v>6</v>
+      </c>
+      <c r="M51" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3632,8 +4138,18 @@
       <c r="H52" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K52" s="3">
+        <v>5</v>
+      </c>
+      <c r="L52" s="3">
+        <v>5</v>
+      </c>
+      <c r="M52" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3658,8 +4174,18 @@
       <c r="H53" s="4" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K53" s="3">
+        <v>9</v>
+      </c>
+      <c r="L53" s="3">
+        <v>9</v>
+      </c>
+      <c r="M53" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3684,8 +4210,18 @@
       <c r="H54" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K54" s="3">
+        <v>12</v>
+      </c>
+      <c r="L54" s="3">
+        <v>13</v>
+      </c>
+      <c r="M54" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3716,8 +4252,18 @@
       <c r="J55" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K55" s="3">
+        <v>12</v>
+      </c>
+      <c r="L55" s="3">
+        <v>11</v>
+      </c>
+      <c r="M55" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3739,8 +4285,18 @@
       <c r="H56" s="4" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K56" s="3">
+        <v>2</v>
+      </c>
+      <c r="L56" s="3">
+        <v>2</v>
+      </c>
+      <c r="M56" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3765,8 +4321,18 @@
       <c r="H57" s="4" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K57" s="3">
+        <v>8</v>
+      </c>
+      <c r="L57" s="3">
+        <v>8</v>
+      </c>
+      <c r="M57" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3791,8 +4357,18 @@
       <c r="H58" s="4" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K58" s="3">
+        <v>2</v>
+      </c>
+      <c r="L58" s="3">
+        <v>2</v>
+      </c>
+      <c r="M58" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3823,8 +4399,18 @@
       <c r="J59" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3">
+        <v>9</v>
+      </c>
+      <c r="L59" s="3">
+        <v>9</v>
+      </c>
+      <c r="M59" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3846,8 +4432,18 @@
       <c r="H60" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K60" s="3">
+        <v>2</v>
+      </c>
+      <c r="L60" s="3">
+        <v>2</v>
+      </c>
+      <c r="M60" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3869,8 +4465,18 @@
       <c r="H61" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K61" s="3">
+        <v>5</v>
+      </c>
+      <c r="L61" s="3">
+        <v>5</v>
+      </c>
+      <c r="M61" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3895,8 +4501,18 @@
       <c r="H62" s="4" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K62" s="3">
+        <v>4</v>
+      </c>
+      <c r="L62" s="3">
+        <v>4</v>
+      </c>
+      <c r="M62" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3918,8 +4534,18 @@
       <c r="H63" s="4" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K63" s="3">
+        <v>10</v>
+      </c>
+      <c r="L63" s="3">
+        <v>11</v>
+      </c>
+      <c r="M63" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -3950,8 +4576,18 @@
       <c r="J64" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K64" s="3">
+        <v>9</v>
+      </c>
+      <c r="L64" s="3">
+        <v>8</v>
+      </c>
+      <c r="M64" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -3973,8 +4609,18 @@
       <c r="H65" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K65" s="3">
+        <v>10</v>
+      </c>
+      <c r="L65" s="3">
+        <v>10</v>
+      </c>
+      <c r="M65" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4005,8 +4651,18 @@
       <c r="J66" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K66" s="3">
+        <v>5</v>
+      </c>
+      <c r="L66" s="3">
+        <v>6</v>
+      </c>
+      <c r="M66" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4031,8 +4687,18 @@
       <c r="H67" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K67" s="3">
+        <v>6</v>
+      </c>
+      <c r="L67" s="3">
+        <v>6</v>
+      </c>
+      <c r="M67" s="3">
+        <f t="shared" ref="M67:M130" si="1">_xlfn.CEILING.MATH(AVERAGE(K67,L67))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4063,8 +4729,18 @@
       <c r="J68" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K68" s="3">
+        <v>10</v>
+      </c>
+      <c r="L68" s="3">
+        <v>10</v>
+      </c>
+      <c r="M68" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4095,8 +4771,18 @@
       <c r="J69" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K69" s="3">
+        <v>9</v>
+      </c>
+      <c r="L69" s="3">
+        <v>9</v>
+      </c>
+      <c r="M69" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4127,8 +4813,18 @@
       <c r="J70" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K70" s="3">
+        <v>8</v>
+      </c>
+      <c r="L70" s="3">
+        <v>8</v>
+      </c>
+      <c r="M70" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4153,8 +4849,18 @@
       <c r="H71" s="4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K71" s="3">
+        <v>2</v>
+      </c>
+      <c r="L71" s="3">
+        <v>7</v>
+      </c>
+      <c r="M71" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4185,8 +4891,18 @@
       <c r="J72" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K72" s="3">
+        <v>9</v>
+      </c>
+      <c r="L72" s="3">
+        <v>9</v>
+      </c>
+      <c r="M72" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4217,8 +4933,18 @@
       <c r="J73" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K73" s="3">
+        <v>2</v>
+      </c>
+      <c r="L73" s="3">
+        <v>2</v>
+      </c>
+      <c r="M73" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4249,8 +4975,18 @@
       <c r="J74" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K74" s="3">
+        <v>7</v>
+      </c>
+      <c r="L74" s="3">
+        <v>7</v>
+      </c>
+      <c r="M74" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4281,8 +5017,18 @@
       <c r="J75" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="3">
+        <v>10</v>
+      </c>
+      <c r="L75" s="3">
+        <v>10</v>
+      </c>
+      <c r="M75" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4307,8 +5053,18 @@
       <c r="H76" s="4" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K76" s="3">
+        <v>12</v>
+      </c>
+      <c r="L76" s="3">
+        <v>11</v>
+      </c>
+      <c r="M76" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4339,8 +5095,18 @@
       <c r="J77" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K77" s="3">
+        <v>4</v>
+      </c>
+      <c r="L77" s="3">
+        <v>4</v>
+      </c>
+      <c r="M77" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -4371,8 +5137,18 @@
       <c r="J78" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K78" s="3">
+        <v>12</v>
+      </c>
+      <c r="L78" s="3">
+        <v>12</v>
+      </c>
+      <c r="M78" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -4403,8 +5179,18 @@
       <c r="J79" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K79" s="3">
+        <v>5</v>
+      </c>
+      <c r="L79" s="3">
+        <v>5</v>
+      </c>
+      <c r="M79" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -4435,8 +5221,18 @@
       <c r="J80" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K80" s="3">
+        <v>8</v>
+      </c>
+      <c r="L80" s="3">
+        <v>8</v>
+      </c>
+      <c r="M80" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -4461,8 +5257,18 @@
       <c r="H81" s="4" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K81" s="3">
+        <v>6</v>
+      </c>
+      <c r="L81" s="3">
+        <v>9</v>
+      </c>
+      <c r="M81" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -4487,8 +5293,18 @@
       <c r="H82" s="4" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K82" s="3">
+        <v>9</v>
+      </c>
+      <c r="L82" s="3">
+        <v>9</v>
+      </c>
+      <c r="M82" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -4513,8 +5329,18 @@
       <c r="H83" s="4" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K83" s="3">
+        <v>2</v>
+      </c>
+      <c r="L83" s="3">
+        <v>2</v>
+      </c>
+      <c r="M83" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -4536,8 +5362,18 @@
       <c r="H84" s="4" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K84" s="3">
+        <v>2</v>
+      </c>
+      <c r="L84" s="3">
+        <v>2</v>
+      </c>
+      <c r="M84" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -4568,8 +5404,18 @@
       <c r="J85" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="3">
+        <v>11</v>
+      </c>
+      <c r="L85" s="3">
+        <v>11</v>
+      </c>
+      <c r="M85" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -4591,8 +5437,18 @@
       <c r="H86" s="4" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K86" s="3">
+        <v>11</v>
+      </c>
+      <c r="L86" s="3">
+        <v>11</v>
+      </c>
+      <c r="M86" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -4623,8 +5479,18 @@
       <c r="J87" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K87" s="3">
+        <v>15</v>
+      </c>
+      <c r="L87" s="3">
+        <v>15</v>
+      </c>
+      <c r="M87" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -4655,8 +5521,18 @@
       <c r="J88" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K88" s="3">
+        <v>10</v>
+      </c>
+      <c r="L88" s="3">
+        <v>10</v>
+      </c>
+      <c r="M88" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -4684,8 +5560,18 @@
       <c r="J89" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K89" s="3">
+        <v>9</v>
+      </c>
+      <c r="L89" s="3">
+        <v>9</v>
+      </c>
+      <c r="M89" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -4707,8 +5593,18 @@
       <c r="H90" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="3">
+        <v>4</v>
+      </c>
+      <c r="L90" s="3">
+        <v>5</v>
+      </c>
+      <c r="M90" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -4730,8 +5626,18 @@
       <c r="H91" s="4" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K91" s="3">
+        <v>9</v>
+      </c>
+      <c r="L91" s="3">
+        <v>9</v>
+      </c>
+      <c r="M91" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -4756,8 +5662,18 @@
       <c r="H92" s="4" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K92" s="3">
+        <v>2</v>
+      </c>
+      <c r="L92" s="3">
+        <v>2</v>
+      </c>
+      <c r="M92" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -4788,8 +5704,18 @@
       <c r="J93" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K93" s="3">
+        <v>9</v>
+      </c>
+      <c r="L93" s="3">
+        <v>9</v>
+      </c>
+      <c r="M93" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -4820,8 +5746,18 @@
       <c r="J94" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K94" s="3">
+        <v>6</v>
+      </c>
+      <c r="L94" s="3">
+        <v>6</v>
+      </c>
+      <c r="M94" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -4846,8 +5782,18 @@
       <c r="H95" s="4" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K95" s="3">
+        <v>2</v>
+      </c>
+      <c r="L95" s="3">
+        <v>2</v>
+      </c>
+      <c r="M95" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -4878,8 +5824,18 @@
       <c r="J96" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K96" s="3">
+        <v>6</v>
+      </c>
+      <c r="L96" s="3">
+        <v>6</v>
+      </c>
+      <c r="M96" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -4910,8 +5866,18 @@
       <c r="J97" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K97" s="3">
+        <v>11</v>
+      </c>
+      <c r="L97" s="3">
+        <v>11</v>
+      </c>
+      <c r="M97" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -4942,8 +5908,18 @@
       <c r="J98" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K98" s="3">
+        <v>8</v>
+      </c>
+      <c r="L98" s="3">
+        <v>8</v>
+      </c>
+      <c r="M98" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -4968,8 +5944,18 @@
       <c r="H99" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K99" s="3">
+        <v>12</v>
+      </c>
+      <c r="L99" s="3">
+        <v>14</v>
+      </c>
+      <c r="M99" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -5000,8 +5986,18 @@
       <c r="J100" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K100" s="3">
+        <v>9</v>
+      </c>
+      <c r="L100" s="3">
+        <v>9</v>
+      </c>
+      <c r="M100" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -5026,8 +6022,18 @@
       <c r="H101" s="4" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K101" s="3">
+        <v>9</v>
+      </c>
+      <c r="L101" s="3">
+        <v>9</v>
+      </c>
+      <c r="M101" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -5058,8 +6064,18 @@
       <c r="J102" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K102" s="3">
+        <v>7</v>
+      </c>
+      <c r="L102" s="3">
+        <v>7</v>
+      </c>
+      <c r="M102" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -5084,8 +6100,18 @@
       <c r="H103" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="3">
+        <v>10</v>
+      </c>
+      <c r="L103" s="3">
+        <v>10</v>
+      </c>
+      <c r="M103" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -5107,8 +6133,18 @@
       <c r="H104" s="4" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K104" s="3">
+        <v>6</v>
+      </c>
+      <c r="L104" s="3">
+        <v>6</v>
+      </c>
+      <c r="M104" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -5133,8 +6169,18 @@
       <c r="J105" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K105" s="3">
+        <v>14</v>
+      </c>
+      <c r="L105" s="3">
+        <v>14</v>
+      </c>
+      <c r="M105" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -5165,8 +6211,18 @@
       <c r="J106" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K106" s="3">
+        <v>9</v>
+      </c>
+      <c r="L106" s="3">
+        <v>9</v>
+      </c>
+      <c r="M106" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -5188,8 +6244,18 @@
       <c r="H107" s="4" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K107" s="3">
+        <v>11</v>
+      </c>
+      <c r="L107" s="3">
+        <v>11</v>
+      </c>
+      <c r="M107" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -5220,8 +6286,18 @@
       <c r="J108" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108" s="3">
+        <v>11</v>
+      </c>
+      <c r="L108" s="3">
+        <v>11</v>
+      </c>
+      <c r="M108" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -5243,8 +6319,18 @@
       <c r="H109" s="4" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K109" s="3">
+        <v>5</v>
+      </c>
+      <c r="L109" s="3">
+        <v>5</v>
+      </c>
+      <c r="M109" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -5269,8 +6355,18 @@
       <c r="H110" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K110" s="3">
+        <v>12</v>
+      </c>
+      <c r="L110" s="3">
+        <v>12</v>
+      </c>
+      <c r="M110" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -5301,8 +6397,18 @@
       <c r="J111" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K111" s="3">
+        <v>9</v>
+      </c>
+      <c r="L111" s="3">
+        <v>9</v>
+      </c>
+      <c r="M111" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -5333,8 +6439,18 @@
       <c r="J112" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K112" s="3">
+        <v>8</v>
+      </c>
+      <c r="L112" s="3">
+        <v>8</v>
+      </c>
+      <c r="M112" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -5362,8 +6478,18 @@
       <c r="J113" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K113" s="3">
+        <v>5</v>
+      </c>
+      <c r="L113" s="3">
+        <v>5</v>
+      </c>
+      <c r="M113" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -5385,8 +6511,18 @@
       <c r="H114" s="4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K114" s="3">
+        <v>11</v>
+      </c>
+      <c r="L114" s="3">
+        <v>11</v>
+      </c>
+      <c r="M114" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -5411,8 +6547,18 @@
       <c r="H115" s="4" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K115" s="3">
+        <v>8</v>
+      </c>
+      <c r="L115" s="3">
+        <v>8</v>
+      </c>
+      <c r="M115" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -5434,8 +6580,18 @@
       <c r="H116" s="4" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K116" s="3">
+        <v>2</v>
+      </c>
+      <c r="L116" s="3">
+        <v>2</v>
+      </c>
+      <c r="M116" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -5466,8 +6622,18 @@
       <c r="J117" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K117" s="3">
+        <v>9</v>
+      </c>
+      <c r="L117" s="3">
+        <v>9</v>
+      </c>
+      <c r="M117" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -5489,8 +6655,18 @@
       <c r="H118" s="4" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K118" s="3">
+        <v>6</v>
+      </c>
+      <c r="L118" s="3">
+        <v>6</v>
+      </c>
+      <c r="M118" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -5512,8 +6688,18 @@
       <c r="H119" s="4" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K119" s="3">
+        <v>2</v>
+      </c>
+      <c r="L119" s="3">
+        <v>2</v>
+      </c>
+      <c r="M119" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -5544,8 +6730,18 @@
       <c r="J120" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K120" s="3">
+        <v>12</v>
+      </c>
+      <c r="L120" s="3">
+        <v>12</v>
+      </c>
+      <c r="M120" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -5576,8 +6772,18 @@
       <c r="J121" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K121" s="3">
+        <v>8</v>
+      </c>
+      <c r="L121" s="3">
+        <v>8</v>
+      </c>
+      <c r="M121" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -5608,8 +6814,18 @@
       <c r="J122" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K122" s="3">
+        <v>8</v>
+      </c>
+      <c r="L122" s="3">
+        <v>9</v>
+      </c>
+      <c r="M122" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -5634,8 +6850,18 @@
       <c r="H123" s="4" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K123" s="3">
+        <v>5</v>
+      </c>
+      <c r="L123" s="3">
+        <v>5</v>
+      </c>
+      <c r="M123" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -5666,8 +6892,18 @@
       <c r="J124" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K124" s="3">
+        <v>10</v>
+      </c>
+      <c r="L124" s="3">
+        <v>10</v>
+      </c>
+      <c r="M124" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -5698,8 +6934,18 @@
       <c r="J125" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K125" s="3">
+        <v>7</v>
+      </c>
+      <c r="L125" s="3">
+        <v>8</v>
+      </c>
+      <c r="M125" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -5730,8 +6976,18 @@
       <c r="J126" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K126" s="3">
+        <v>11</v>
+      </c>
+      <c r="L126" s="3">
+        <v>11</v>
+      </c>
+      <c r="M126" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -5762,8 +7018,18 @@
       <c r="J127" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127" s="3">
+        <v>14</v>
+      </c>
+      <c r="L127" s="3">
+        <v>14</v>
+      </c>
+      <c r="M127" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -5791,8 +7057,18 @@
       <c r="J128" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K128" s="3">
+        <v>8</v>
+      </c>
+      <c r="L128" s="3">
+        <v>8</v>
+      </c>
+      <c r="M128" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -5814,8 +7090,18 @@
       <c r="H129" s="4" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K129" s="3">
+        <v>2</v>
+      </c>
+      <c r="L129" s="3">
+        <v>2</v>
+      </c>
+      <c r="M129" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -5840,8 +7126,18 @@
       <c r="J130" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K130" s="3">
+        <v>6</v>
+      </c>
+      <c r="L130" s="3">
+        <v>7</v>
+      </c>
+      <c r="M130" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -5863,8 +7159,18 @@
       <c r="H131" s="4" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K131" s="3">
+        <v>5</v>
+      </c>
+      <c r="L131" s="3">
+        <v>5</v>
+      </c>
+      <c r="M131" s="3">
+        <f t="shared" ref="M131:M185" si="2">_xlfn.CEILING.MATH(AVERAGE(K131,L131))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -5895,8 +7201,18 @@
       <c r="J132" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K132" s="3">
+        <v>10</v>
+      </c>
+      <c r="L132" s="3">
+        <v>9</v>
+      </c>
+      <c r="M132" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -5927,8 +7243,18 @@
       <c r="J133" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K133" s="3">
+        <v>12</v>
+      </c>
+      <c r="L133" s="3">
+        <v>12</v>
+      </c>
+      <c r="M133" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -5956,8 +7282,18 @@
       <c r="J134" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K134" s="3">
+        <v>5</v>
+      </c>
+      <c r="L134" s="3">
+        <v>5</v>
+      </c>
+      <c r="M134" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -5982,8 +7318,18 @@
       <c r="H135" s="4" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K135" s="3">
+        <v>5</v>
+      </c>
+      <c r="L135" s="3">
+        <v>5</v>
+      </c>
+      <c r="M135" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -6011,8 +7357,18 @@
       <c r="J136" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K136" s="3">
+        <v>7</v>
+      </c>
+      <c r="L136" s="3">
+        <v>8</v>
+      </c>
+      <c r="M136" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -6034,8 +7390,18 @@
       <c r="H137" s="4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K137" s="3">
+        <v>2</v>
+      </c>
+      <c r="L137" s="3">
+        <v>2</v>
+      </c>
+      <c r="M137" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -6066,8 +7432,18 @@
       <c r="J138" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K138" s="3">
+        <v>9</v>
+      </c>
+      <c r="L138" s="3">
+        <v>9</v>
+      </c>
+      <c r="M138" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -6092,8 +7468,18 @@
       <c r="J139" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K139" s="3">
+        <v>14</v>
+      </c>
+      <c r="L139" s="3">
+        <v>14</v>
+      </c>
+      <c r="M139" s="3">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -6115,8 +7501,18 @@
       <c r="H140" s="4" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K140" s="3">
+        <v>10</v>
+      </c>
+      <c r="L140" s="3">
+        <v>11</v>
+      </c>
+      <c r="M140" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -6138,8 +7534,18 @@
       <c r="H141" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K141" s="3">
+        <v>8</v>
+      </c>
+      <c r="L141" s="3">
+        <v>8</v>
+      </c>
+      <c r="M141" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -6161,8 +7567,18 @@
       <c r="H142" s="4" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K142" s="3">
+        <v>2</v>
+      </c>
+      <c r="L142" s="3">
+        <v>2</v>
+      </c>
+      <c r="M142" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -6190,8 +7606,18 @@
       <c r="J143" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K143" s="3">
+        <v>9</v>
+      </c>
+      <c r="L143" s="3">
+        <v>9</v>
+      </c>
+      <c r="M143" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -6222,8 +7648,18 @@
       <c r="J144" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K144" s="3">
+        <v>12</v>
+      </c>
+      <c r="L144" s="3">
+        <v>12</v>
+      </c>
+      <c r="M144" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -6254,8 +7690,18 @@
       <c r="J145" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K145" s="3">
+        <v>11</v>
+      </c>
+      <c r="L145" s="3">
+        <v>11</v>
+      </c>
+      <c r="M145" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -6286,8 +7732,18 @@
       <c r="J146" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K146" s="3">
+        <v>9</v>
+      </c>
+      <c r="L146" s="3">
+        <v>9</v>
+      </c>
+      <c r="M146" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -6312,8 +7768,18 @@
       <c r="H147" s="4" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K147" s="3">
+        <v>8</v>
+      </c>
+      <c r="L147" s="3">
+        <v>8</v>
+      </c>
+      <c r="M147" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -6335,8 +7801,18 @@
       <c r="H148" s="4" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K148" s="3">
+        <v>5</v>
+      </c>
+      <c r="L148" s="3">
+        <v>5</v>
+      </c>
+      <c r="M148" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -6367,8 +7843,18 @@
       <c r="J149" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K149" s="3">
+        <v>11</v>
+      </c>
+      <c r="L149" s="3">
+        <v>11</v>
+      </c>
+      <c r="M149" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -6399,8 +7885,18 @@
       <c r="J150" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K150" s="3">
+        <v>11</v>
+      </c>
+      <c r="L150" s="3">
+        <v>11</v>
+      </c>
+      <c r="M150" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -6431,8 +7927,18 @@
       <c r="J151" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K151" s="3">
+        <v>11</v>
+      </c>
+      <c r="L151" s="3">
+        <v>12</v>
+      </c>
+      <c r="M151" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -6463,8 +7969,18 @@
       <c r="J152" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K152" s="3">
+        <v>12</v>
+      </c>
+      <c r="L152" s="3">
+        <v>12</v>
+      </c>
+      <c r="M152" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -6492,8 +8008,18 @@
       <c r="J153" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K153" s="3">
+        <v>12</v>
+      </c>
+      <c r="L153" s="3">
+        <v>12</v>
+      </c>
+      <c r="M153" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -6524,8 +8050,18 @@
       <c r="J154" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K154" s="3">
+        <v>11</v>
+      </c>
+      <c r="L154" s="3">
+        <v>11</v>
+      </c>
+      <c r="M154" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -6556,8 +8092,18 @@
       <c r="J155" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K155" s="3">
+        <v>9</v>
+      </c>
+      <c r="L155" s="3">
+        <v>9</v>
+      </c>
+      <c r="M155" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -6585,8 +8131,18 @@
       <c r="J156" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K156" s="3">
+        <v>9</v>
+      </c>
+      <c r="L156" s="3">
+        <v>9</v>
+      </c>
+      <c r="M156" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -6614,8 +8170,18 @@
       <c r="J157" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K157" s="3">
+        <v>11</v>
+      </c>
+      <c r="L157" s="3">
+        <v>11</v>
+      </c>
+      <c r="M157" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -6643,8 +8209,18 @@
       <c r="J158" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K158" s="3">
+        <v>12</v>
+      </c>
+      <c r="L158" s="3">
+        <v>12</v>
+      </c>
+      <c r="M158" s="3">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -6672,8 +8248,18 @@
       <c r="J159" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K159" s="3">
+        <v>9</v>
+      </c>
+      <c r="L159" s="3">
+        <v>9</v>
+      </c>
+      <c r="M159" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -6704,8 +8290,18 @@
       <c r="J160" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K160" s="3">
+        <v>8</v>
+      </c>
+      <c r="L160" s="3">
+        <v>8</v>
+      </c>
+      <c r="M160" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -6733,8 +8329,18 @@
       <c r="J161" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K161" s="3">
+        <v>8</v>
+      </c>
+      <c r="L161" s="3">
+        <v>8</v>
+      </c>
+      <c r="M161" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -6759,8 +8365,18 @@
       <c r="H162" s="4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K162" s="3">
+        <v>2</v>
+      </c>
+      <c r="L162" s="3">
+        <v>2</v>
+      </c>
+      <c r="M162" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -6785,8 +8401,18 @@
       <c r="H163" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K163" s="3">
+        <v>5</v>
+      </c>
+      <c r="L163" s="3">
+        <v>5</v>
+      </c>
+      <c r="M163" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -6811,8 +8437,18 @@
       <c r="H164" s="4" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K164" s="3">
+        <v>4</v>
+      </c>
+      <c r="L164" s="3">
+        <v>5</v>
+      </c>
+      <c r="M164" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -6840,8 +8476,18 @@
       <c r="J165" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K165" s="3">
+        <v>9</v>
+      </c>
+      <c r="L165" s="3">
+        <v>9</v>
+      </c>
+      <c r="M165" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -6866,8 +8512,18 @@
       <c r="H166" s="4" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K166" s="3">
+        <v>9</v>
+      </c>
+      <c r="L166" s="3">
+        <v>8</v>
+      </c>
+      <c r="M166" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -6892,8 +8548,18 @@
       <c r="H167" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K167" s="3">
+        <v>9</v>
+      </c>
+      <c r="L167" s="3">
+        <v>9</v>
+      </c>
+      <c r="M167" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -6918,8 +8584,18 @@
       <c r="H168" s="4" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K168" s="3">
+        <v>2</v>
+      </c>
+      <c r="L168" s="3">
+        <v>2</v>
+      </c>
+      <c r="M168" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -6938,8 +8614,18 @@
       <c r="H169" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K169" s="3">
+        <v>8</v>
+      </c>
+      <c r="L169" s="3">
+        <v>8</v>
+      </c>
+      <c r="M169" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -6958,8 +8644,18 @@
       <c r="H170" s="4" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K170" s="3">
+        <v>9</v>
+      </c>
+      <c r="L170" s="3">
+        <v>9</v>
+      </c>
+      <c r="M170" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -6978,8 +8674,18 @@
       <c r="H171" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K171" s="3">
+        <v>8</v>
+      </c>
+      <c r="L171" s="3">
+        <v>8</v>
+      </c>
+      <c r="M171" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -6998,8 +8704,18 @@
       <c r="H172" s="4" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K172" s="3">
+        <v>11</v>
+      </c>
+      <c r="L172" s="3">
+        <v>11</v>
+      </c>
+      <c r="M172" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -7018,8 +8734,18 @@
       <c r="H173" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K173" s="3">
+        <v>10</v>
+      </c>
+      <c r="L173" s="3">
+        <v>9</v>
+      </c>
+      <c r="M173" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -7038,8 +8764,18 @@
       <c r="H174" s="4" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K174" s="3">
+        <v>8</v>
+      </c>
+      <c r="L174" s="3">
+        <v>8</v>
+      </c>
+      <c r="M174" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -7058,8 +8794,18 @@
       <c r="H175" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K175" s="3">
+        <v>11</v>
+      </c>
+      <c r="L175" s="3">
+        <v>11</v>
+      </c>
+      <c r="M175" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -7078,8 +8824,18 @@
       <c r="H176" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K176" s="3">
+        <v>10</v>
+      </c>
+      <c r="L176" s="3">
+        <v>10</v>
+      </c>
+      <c r="M176" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -7098,8 +8854,18 @@
       <c r="H177" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K177" s="3">
+        <v>11</v>
+      </c>
+      <c r="L177" s="3">
+        <v>11</v>
+      </c>
+      <c r="M177" s="3">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -7118,8 +8884,18 @@
       <c r="H178" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K178" s="3">
+        <v>9</v>
+      </c>
+      <c r="L178" s="3">
+        <v>9</v>
+      </c>
+      <c r="M178" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -7138,8 +8914,18 @@
       <c r="H179" s="4" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K179" s="3">
+        <v>8</v>
+      </c>
+      <c r="L179" s="3">
+        <v>8</v>
+      </c>
+      <c r="M179" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -7158,8 +8944,18 @@
       <c r="H180" s="4" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K180" s="3">
+        <v>8</v>
+      </c>
+      <c r="L180" s="3">
+        <v>8</v>
+      </c>
+      <c r="M180" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -7178,8 +8974,18 @@
       <c r="H181" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="K181" s="3">
+        <v>8</v>
+      </c>
+      <c r="L181" s="3">
+        <v>8</v>
+      </c>
+      <c r="M181" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -7198,8 +9004,18 @@
       <c r="H182" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="K182" s="3">
+        <v>2</v>
+      </c>
+      <c r="L182" s="3">
+        <v>2</v>
+      </c>
+      <c r="M182" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -7218,8 +9034,18 @@
       <c r="H183" s="4" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K183" s="3">
+        <v>10</v>
+      </c>
+      <c r="L183" s="3">
+        <v>10</v>
+      </c>
+      <c r="M183" s="3">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -7238,8 +9064,18 @@
       <c r="H184" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K184" s="3">
+        <v>8</v>
+      </c>
+      <c r="L184" s="3">
+        <v>8</v>
+      </c>
+      <c r="M184" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -7257,6 +9093,16 @@
       </c>
       <c r="H185" s="4" t="s">
         <v>247</v>
+      </c>
+      <c r="K185" s="3">
+        <v>8</v>
+      </c>
+      <c r="L185" s="3">
+        <v>8</v>
+      </c>
+      <c r="M185" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -7270,7 +9116,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>